<commit_message>
add translation scripts to the appropriate files (removed from case studies repo). re-run to produce datasets.
</commit_message>
<xml_diff>
--- a/inst/extdata/notificacoes_multidoencas.xlsx
+++ b/inst/extdata/notificacoes_multidoencas.xlsx
@@ -639,7 +639,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Lake Minara</t>
+          <t>Lago Minara</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -840,7 +840,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Lake Minara</t>
+          <t>Lago Minara</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -1255,7 +1255,7 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -1292,7 +1292,7 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
@@ -1491,7 +1491,7 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
@@ -2118,7 +2118,7 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>Lake Minara</t>
+          <t>Lago Minara</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
@@ -2217,7 +2217,7 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>Lake Minara</t>
+          <t>Lago Minara</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
@@ -2274,7 +2274,7 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
@@ -2481,7 +2481,7 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>Lake Minara</t>
+          <t>Lago Minara</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
@@ -2729,7 +2729,7 @@
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
@@ -3037,7 +3037,7 @@
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>Lake Minara</t>
+          <t>Lago Minara</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
@@ -3139,7 +3139,7 @@
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H55" t="inlineStr">
@@ -3452,7 +3452,7 @@
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H61" t="inlineStr">
@@ -3549,7 +3549,7 @@
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>Lake Minara</t>
+          <t>Lago Minara</t>
         </is>
       </c>
       <c r="H63" t="inlineStr">
@@ -3651,7 +3651,7 @@
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H65" t="inlineStr">
@@ -3805,7 +3805,7 @@
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H68" t="inlineStr">
@@ -4207,7 +4207,7 @@
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H76" t="inlineStr">
@@ -4254,7 +4254,7 @@
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H77" t="inlineStr">
@@ -4309,7 +4309,7 @@
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H78" t="inlineStr">
@@ -4523,7 +4523,7 @@
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H82" t="inlineStr">
@@ -4685,7 +4685,7 @@
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>Lake Minara</t>
+          <t>Lago Minara</t>
         </is>
       </c>
       <c r="H85" t="inlineStr">
@@ -4740,7 +4740,7 @@
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>Lake Minara</t>
+          <t>Lago Minara</t>
         </is>
       </c>
       <c r="H86" t="inlineStr">
@@ -4849,7 +4849,7 @@
       </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H88" t="inlineStr">
@@ -5102,7 +5102,7 @@
       </c>
       <c r="G93" t="inlineStr">
         <is>
-          <t>Lake Minara</t>
+          <t>Lago Minara</t>
         </is>
       </c>
       <c r="H93" t="inlineStr">
@@ -5497,7 +5497,7 @@
       </c>
       <c r="G101" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H101" t="inlineStr">
@@ -5549,7 +5549,7 @@
       </c>
       <c r="G102" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H102" t="inlineStr">
@@ -5648,7 +5648,7 @@
       </c>
       <c r="G104" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H104" t="inlineStr">
@@ -5963,7 +5963,7 @@
       </c>
       <c r="G110" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H110" t="inlineStr">
@@ -6170,7 +6170,7 @@
       </c>
       <c r="G114" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H114" t="inlineStr">
@@ -6222,7 +6222,7 @@
       </c>
       <c r="G115" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H115" t="inlineStr">
@@ -6326,7 +6326,7 @@
       </c>
       <c r="G117" t="inlineStr">
         <is>
-          <t>Lake Minara</t>
+          <t>Lago Minara</t>
         </is>
       </c>
       <c r="H117" t="inlineStr">
@@ -6577,7 +6577,7 @@
       </c>
       <c r="G122" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H122" t="inlineStr">
@@ -6729,7 +6729,7 @@
       </c>
       <c r="G125" t="inlineStr">
         <is>
-          <t>Lake Minara</t>
+          <t>Lago Minara</t>
         </is>
       </c>
       <c r="H125" t="inlineStr">
@@ -7210,7 +7210,7 @@
       </c>
       <c r="G134" t="inlineStr">
         <is>
-          <t>Lake Minara</t>
+          <t>Lago Minara</t>
         </is>
       </c>
       <c r="H134" t="inlineStr">
@@ -7801,7 +7801,7 @@
       </c>
       <c r="G145" t="inlineStr">
         <is>
-          <t>Lake Minara</t>
+          <t>Lago Minara</t>
         </is>
       </c>
       <c r="H145" t="inlineStr">
@@ -7851,7 +7851,7 @@
       </c>
       <c r="G146" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H146" t="inlineStr">
@@ -7903,7 +7903,7 @@
       </c>
       <c r="G147" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H147" t="inlineStr">
@@ -8055,7 +8055,7 @@
       </c>
       <c r="G150" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H150" t="inlineStr">
@@ -8385,7 +8385,7 @@
       </c>
       <c r="G157" t="inlineStr">
         <is>
-          <t>Lake Minara</t>
+          <t>Lago Minara</t>
         </is>
       </c>
       <c r="H157" t="inlineStr">
@@ -8529,7 +8529,7 @@
       </c>
       <c r="G160" t="inlineStr">
         <is>
-          <t>Lake Minara</t>
+          <t>Lago Minara</t>
         </is>
       </c>
       <c r="H160" t="inlineStr">
@@ -8694,7 +8694,7 @@
       </c>
       <c r="G163" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H163" t="inlineStr">
@@ -8749,7 +8749,7 @@
       </c>
       <c r="G164" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H164" t="inlineStr">
@@ -8844,7 +8844,7 @@
       </c>
       <c r="G166" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H166" t="inlineStr">
@@ -8936,7 +8936,7 @@
       </c>
       <c r="G168" t="inlineStr">
         <is>
-          <t>Lake Minara</t>
+          <t>Lago Minara</t>
         </is>
       </c>
       <c r="H168" t="inlineStr">
@@ -9143,7 +9143,7 @@
       </c>
       <c r="G172" t="inlineStr">
         <is>
-          <t>Lake Minara</t>
+          <t>Lago Minara</t>
         </is>
       </c>
       <c r="H172" t="inlineStr">
@@ -9190,7 +9190,7 @@
       </c>
       <c r="G173" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H173" t="inlineStr">
@@ -9496,7 +9496,7 @@
       </c>
       <c r="G179" t="inlineStr">
         <is>
-          <t>Lake Minara</t>
+          <t>Lago Minara</t>
         </is>
       </c>
       <c r="H179" t="inlineStr">
@@ -9533,7 +9533,7 @@
       </c>
       <c r="G180" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H180" t="inlineStr">
@@ -9593,7 +9593,7 @@
       </c>
       <c r="G181" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H181" t="inlineStr">
@@ -9742,7 +9742,7 @@
       </c>
       <c r="G184" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H184" t="inlineStr">
@@ -9978,7 +9978,7 @@
       </c>
       <c r="G189" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H189" t="inlineStr">
@@ -10180,7 +10180,7 @@
       </c>
       <c r="G193" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H193" t="inlineStr">
@@ -10284,7 +10284,7 @@
       </c>
       <c r="G195" t="inlineStr">
         <is>
-          <t>Lake Minara</t>
+          <t>Lago Minara</t>
         </is>
       </c>
       <c r="H195" t="inlineStr">
@@ -10329,7 +10329,7 @@
       </c>
       <c r="G196" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H196" t="inlineStr">
@@ -10501,7 +10501,7 @@
       </c>
       <c r="G199" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H199" t="inlineStr">
@@ -10695,7 +10695,7 @@
       </c>
       <c r="G203" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H203" t="inlineStr">
@@ -10947,7 +10947,7 @@
       </c>
       <c r="G208" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H208" t="inlineStr">
@@ -10989,7 +10989,7 @@
       </c>
       <c r="G209" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H209" t="inlineStr">
@@ -11361,7 +11361,7 @@
       </c>
       <c r="G216" t="inlineStr">
         <is>
-          <t>Lake Minara</t>
+          <t>Lago Minara</t>
         </is>
       </c>
       <c r="H216" t="inlineStr">
@@ -11401,7 +11401,7 @@
       </c>
       <c r="G217" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H217" t="inlineStr">
@@ -11453,7 +11453,7 @@
       </c>
       <c r="G218" t="inlineStr">
         <is>
-          <t>Lake Minara</t>
+          <t>Lago Minara</t>
         </is>
       </c>
       <c r="H218" t="inlineStr">
@@ -11505,7 +11505,7 @@
       </c>
       <c r="G219" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H219" t="inlineStr">
@@ -11595,7 +11595,7 @@
       </c>
       <c r="G221" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H221" t="inlineStr">
@@ -11700,7 +11700,7 @@
       </c>
       <c r="G223" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H223" t="inlineStr">
@@ -11799,7 +11799,7 @@
       </c>
       <c r="G225" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H225" t="inlineStr">
@@ -12137,7 +12137,7 @@
       </c>
       <c r="G231" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H231" t="inlineStr">
@@ -12399,7 +12399,7 @@
       </c>
       <c r="G236" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H236" t="inlineStr">
@@ -12663,7 +12663,7 @@
       </c>
       <c r="G241" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H241" t="inlineStr">
@@ -12977,7 +12977,7 @@
       </c>
       <c r="G247" t="inlineStr">
         <is>
-          <t>Lake Minara</t>
+          <t>Lago Minara</t>
         </is>
       </c>
       <c r="H247" t="inlineStr">
@@ -13064,7 +13064,7 @@
       </c>
       <c r="G249" t="inlineStr">
         <is>
-          <t>Lake Minara</t>
+          <t>Lago Minara</t>
         </is>
       </c>
       <c r="H249" t="inlineStr">
@@ -13262,7 +13262,7 @@
       </c>
       <c r="G253" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H253" t="inlineStr">
@@ -13416,7 +13416,7 @@
       </c>
       <c r="G256" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H256" t="inlineStr">
@@ -13672,7 +13672,7 @@
       </c>
       <c r="G261" t="inlineStr">
         <is>
-          <t>Lake Minara</t>
+          <t>Lago Minara</t>
         </is>
       </c>
       <c r="H261" t="inlineStr">
@@ -13722,7 +13722,7 @@
       </c>
       <c r="G262" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H262" t="inlineStr">
@@ -13777,7 +13777,7 @@
       </c>
       <c r="G263" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H263" t="inlineStr">
@@ -13889,7 +13889,7 @@
       </c>
       <c r="G265" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H265" t="inlineStr">
@@ -14391,7 +14391,7 @@
       </c>
       <c r="G274" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H274" t="inlineStr">
@@ -14503,7 +14503,7 @@
       </c>
       <c r="G276" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H276" t="inlineStr">
@@ -14660,7 +14660,7 @@
       </c>
       <c r="G279" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H279" t="inlineStr">
@@ -14765,7 +14765,7 @@
       </c>
       <c r="G281" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H281" t="inlineStr">
@@ -14822,7 +14822,7 @@
       </c>
       <c r="G282" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H282" t="inlineStr">
@@ -14999,7 +14999,7 @@
       </c>
       <c r="G285" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H285" t="inlineStr">
@@ -15201,7 +15201,7 @@
       </c>
       <c r="G289" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H289" t="inlineStr">
@@ -15397,7 +15397,7 @@
       </c>
       <c r="G293" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H293" t="inlineStr">
@@ -15489,7 +15489,7 @@
       </c>
       <c r="G295" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H295" t="inlineStr">
@@ -15862,7 +15862,7 @@
       </c>
       <c r="G302" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H302" t="inlineStr">
@@ -15949,7 +15949,7 @@
       </c>
       <c r="G304" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H304" t="inlineStr">
@@ -16105,7 +16105,7 @@
       </c>
       <c r="G307" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H307" t="inlineStr">
@@ -16244,7 +16244,7 @@
       </c>
       <c r="G310" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H310" t="inlineStr">
@@ -16401,7 +16401,7 @@
       </c>
       <c r="G313" t="inlineStr">
         <is>
-          <t>Lake Minara</t>
+          <t>Lago Minara</t>
         </is>
       </c>
       <c r="H313" t="inlineStr">
@@ -16446,7 +16446,7 @@
       </c>
       <c r="G314" t="inlineStr">
         <is>
-          <t>Lake Minara</t>
+          <t>Lago Minara</t>
         </is>
       </c>
       <c r="H314" t="inlineStr">
@@ -16600,7 +16600,7 @@
       </c>
       <c r="G317" t="inlineStr">
         <is>
-          <t>Lake Minara</t>
+          <t>Lago Minara</t>
         </is>
       </c>
       <c r="H317" t="inlineStr">
@@ -16752,7 +16752,7 @@
       </c>
       <c r="G320" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H320" t="inlineStr">
@@ -16794,7 +16794,7 @@
       </c>
       <c r="G321" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H321" t="inlineStr">
@@ -16846,7 +16846,7 @@
       </c>
       <c r="G322" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H322" t="inlineStr">
@@ -16898,7 +16898,7 @@
       </c>
       <c r="G323" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H323" t="inlineStr">
@@ -16945,7 +16945,7 @@
       </c>
       <c r="G324" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H324" t="inlineStr">
@@ -17206,7 +17206,7 @@
       </c>
       <c r="G329" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H329" t="inlineStr">
@@ -17958,7 +17958,7 @@
       </c>
       <c r="G343" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H343" t="inlineStr">
@@ -18070,7 +18070,7 @@
       </c>
       <c r="G345" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H345" t="inlineStr">
@@ -18184,7 +18184,7 @@
       </c>
       <c r="G347" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H347" t="inlineStr">
@@ -18284,7 +18284,7 @@
       </c>
       <c r="G349" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H349" t="inlineStr">
@@ -18391,7 +18391,7 @@
       </c>
       <c r="G351" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H351" t="inlineStr">
@@ -18963,7 +18963,7 @@
       </c>
       <c r="G362" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H362" t="inlineStr">
@@ -19008,7 +19008,7 @@
       </c>
       <c r="G363" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H363" t="inlineStr">
@@ -19484,7 +19484,7 @@
       </c>
       <c r="G372" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H372" t="inlineStr">
@@ -19896,7 +19896,7 @@
       </c>
       <c r="G380" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H380" t="inlineStr">
@@ -19928,7 +19928,7 @@
       </c>
       <c r="G381" t="inlineStr">
         <is>
-          <t>Lake Minara</t>
+          <t>Lago Minara</t>
         </is>
       </c>
       <c r="H381" t="inlineStr">
@@ -19983,7 +19983,7 @@
       </c>
       <c r="G382" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H382" t="inlineStr">
@@ -20190,7 +20190,7 @@
       </c>
       <c r="G386" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H386" t="inlineStr">
@@ -20352,7 +20352,7 @@
       </c>
       <c r="G389" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H389" t="inlineStr">
@@ -20404,7 +20404,7 @@
       </c>
       <c r="G390" t="inlineStr">
         <is>
-          <t>Lake Minara</t>
+          <t>Lago Minara</t>
         </is>
       </c>
       <c r="H390" t="inlineStr">
@@ -20451,7 +20451,7 @@
       </c>
       <c r="G391" t="inlineStr">
         <is>
-          <t>Lake Minara</t>
+          <t>Lago Minara</t>
         </is>
       </c>
       <c r="H391" t="inlineStr">
@@ -20561,7 +20561,7 @@
       </c>
       <c r="G393" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H393" t="inlineStr">
@@ -20695,7 +20695,7 @@
       </c>
       <c r="G396" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H396" t="inlineStr">
@@ -20948,7 +20948,7 @@
       </c>
       <c r="G401" t="inlineStr">
         <is>
-          <t>Lake Minara</t>
+          <t>Lago Minara</t>
         </is>
       </c>
       <c r="H401" t="inlineStr">
@@ -21329,7 +21329,7 @@
       </c>
       <c r="G408" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H408" t="inlineStr">
@@ -21548,7 +21548,7 @@
       </c>
       <c r="G412" t="inlineStr">
         <is>
-          <t>Lake Minara</t>
+          <t>Lago Minara</t>
         </is>
       </c>
       <c r="H412" t="inlineStr">
@@ -22194,7 +22194,7 @@
       </c>
       <c r="G424" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H424" t="inlineStr">
@@ -22401,7 +22401,7 @@
       </c>
       <c r="G428" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H428" t="inlineStr">
@@ -22446,7 +22446,7 @@
       </c>
       <c r="G429" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H429" t="inlineStr">
@@ -22561,7 +22561,7 @@
       </c>
       <c r="G431" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H431" t="inlineStr">
@@ -22621,7 +22621,7 @@
       </c>
       <c r="G432" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H432" t="inlineStr">
@@ -22673,7 +22673,7 @@
       </c>
       <c r="G433" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H433" t="inlineStr">
@@ -22820,7 +22820,7 @@
       </c>
       <c r="G436" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H436" t="inlineStr">
@@ -22875,7 +22875,7 @@
       </c>
       <c r="G437" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H437" t="inlineStr">
@@ -22927,7 +22927,7 @@
       </c>
       <c r="G438" t="inlineStr">
         <is>
-          <t>Lake Minara</t>
+          <t>Lago Minara</t>
         </is>
       </c>
       <c r="H438" t="inlineStr">
@@ -23096,7 +23096,7 @@
       </c>
       <c r="G441" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H441" t="inlineStr">
@@ -23148,7 +23148,7 @@
       </c>
       <c r="G442" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H442" t="inlineStr">
@@ -23198,7 +23198,7 @@
       </c>
       <c r="G443" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H443" t="inlineStr">
@@ -23355,7 +23355,7 @@
       </c>
       <c r="G446" t="inlineStr">
         <is>
-          <t>Lake Minara</t>
+          <t>Lago Minara</t>
         </is>
       </c>
       <c r="H446" t="inlineStr">
@@ -23519,7 +23519,7 @@
       </c>
       <c r="G449" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H449" t="inlineStr">
@@ -23571,7 +23571,7 @@
       </c>
       <c r="G450" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H450" t="inlineStr">
@@ -23873,7 +23873,7 @@
       </c>
       <c r="G456" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H456" t="inlineStr">
@@ -24406,7 +24406,7 @@
       </c>
       <c r="G466" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H466" t="inlineStr">
@@ -24934,7 +24934,7 @@
       </c>
       <c r="G476" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H476" t="inlineStr">
@@ -25076,7 +25076,7 @@
       </c>
       <c r="G479" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H479" t="inlineStr">
@@ -25369,7 +25369,7 @@
       </c>
       <c r="G485" t="inlineStr">
         <is>
-          <t>Lake Minara</t>
+          <t>Lago Minara</t>
         </is>
       </c>
       <c r="H485" t="inlineStr">
@@ -26045,7 +26045,7 @@
       </c>
       <c r="G498" t="inlineStr">
         <is>
-          <t>Lake Minara</t>
+          <t>Lago Minara</t>
         </is>
       </c>
       <c r="H498" t="inlineStr">
@@ -26152,7 +26152,7 @@
       </c>
       <c r="G500" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H500" t="inlineStr">
@@ -26408,7 +26408,7 @@
       </c>
       <c r="G505" t="inlineStr">
         <is>
-          <t>Lake Minara</t>
+          <t>Lago Minara</t>
         </is>
       </c>
       <c r="H505" t="inlineStr">
@@ -26453,7 +26453,7 @@
       </c>
       <c r="G506" t="inlineStr">
         <is>
-          <t>Lake Minara</t>
+          <t>Lago Minara</t>
         </is>
       </c>
       <c r="H506" t="inlineStr">
@@ -26508,7 +26508,7 @@
       </c>
       <c r="G507" t="inlineStr">
         <is>
-          <t>Lake Minara</t>
+          <t>Lago Minara</t>
         </is>
       </c>
       <c r="H507" t="inlineStr">
@@ -26718,7 +26718,7 @@
       </c>
       <c r="G511" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H511" t="inlineStr">
@@ -26770,7 +26770,7 @@
       </c>
       <c r="G512" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H512" t="inlineStr">
@@ -26882,7 +26882,7 @@
       </c>
       <c r="G514" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H514" t="inlineStr">
@@ -27491,7 +27491,7 @@
       </c>
       <c r="G526" t="inlineStr">
         <is>
-          <t>Lake Minara</t>
+          <t>Lago Minara</t>
         </is>
       </c>
       <c r="H526" t="inlineStr">
@@ -27578,7 +27578,7 @@
       </c>
       <c r="G528" t="inlineStr">
         <is>
-          <t>Lake Minara</t>
+          <t>Lago Minara</t>
         </is>
       </c>
       <c r="H528" t="inlineStr">
@@ -27888,7 +27888,7 @@
       </c>
       <c r="G534" t="inlineStr">
         <is>
-          <t>Lake Minara</t>
+          <t>Lago Minara</t>
         </is>
       </c>
       <c r="H534" t="inlineStr">
@@ -28045,7 +28045,7 @@
       </c>
       <c r="G537" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H537" t="inlineStr">
@@ -28092,7 +28092,7 @@
       </c>
       <c r="G538" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H538" t="inlineStr">
@@ -28147,7 +28147,7 @@
       </c>
       <c r="G539" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H539" t="inlineStr">
@@ -28194,7 +28194,7 @@
       </c>
       <c r="G540" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H540" t="inlineStr">
@@ -28350,7 +28350,7 @@
       </c>
       <c r="G543" t="inlineStr">
         <is>
-          <t>Lake Minara</t>
+          <t>Lago Minara</t>
         </is>
       </c>
       <c r="H543" t="inlineStr">
@@ -28454,7 +28454,7 @@
       </c>
       <c r="G545" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H545" t="inlineStr">
@@ -29209,7 +29209,7 @@
       </c>
       <c r="G559" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H559" t="inlineStr">
@@ -29283,7 +29283,7 @@
       </c>
       <c r="G561" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H561" t="inlineStr">
@@ -29333,7 +29333,7 @@
       </c>
       <c r="G562" t="inlineStr">
         <is>
-          <t>Lake Minara</t>
+          <t>Lago Minara</t>
         </is>
       </c>
       <c r="H562" t="inlineStr">
@@ -29393,7 +29393,7 @@
       </c>
       <c r="G563" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H563" t="inlineStr">
@@ -29741,7 +29741,7 @@
       </c>
       <c r="G570" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H570" t="inlineStr">
@@ -29940,7 +29940,7 @@
       </c>
       <c r="G574" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H574" t="inlineStr">
@@ -29997,7 +29997,7 @@
       </c>
       <c r="G575" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H575" t="inlineStr">
@@ -30044,7 +30044,7 @@
       </c>
       <c r="G576" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H576" t="inlineStr">
@@ -30091,7 +30091,7 @@
       </c>
       <c r="G577" t="inlineStr">
         <is>
-          <t>Lake Minara</t>
+          <t>Lago Minara</t>
         </is>
       </c>
       <c r="H577" t="inlineStr">
@@ -30692,7 +30692,7 @@
       </c>
       <c r="G589" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H589" t="inlineStr">
@@ -30886,7 +30886,7 @@
       </c>
       <c r="G593" t="inlineStr">
         <is>
-          <t>Lake Minara</t>
+          <t>Lago Minara</t>
         </is>
       </c>
       <c r="H593" t="inlineStr">
@@ -31053,7 +31053,7 @@
       </c>
       <c r="G596" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H596" t="inlineStr">
@@ -31098,7 +31098,7 @@
       </c>
       <c r="G597" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H597" t="inlineStr">
@@ -31148,7 +31148,7 @@
       </c>
       <c r="G598" t="inlineStr">
         <is>
-          <t>Lake Minara</t>
+          <t>Lago Minara</t>
         </is>
       </c>
       <c r="H598" t="inlineStr">
@@ -31200,7 +31200,7 @@
       </c>
       <c r="G599" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H599" t="inlineStr">
@@ -31582,7 +31582,7 @@
       </c>
       <c r="G606" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H606" t="inlineStr">
@@ -31627,7 +31627,7 @@
       </c>
       <c r="G607" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H607" t="inlineStr">
@@ -31938,7 +31938,7 @@
       </c>
       <c r="G613" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H613" t="inlineStr">
@@ -31995,7 +31995,7 @@
       </c>
       <c r="G614" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H614" t="inlineStr">
@@ -32097,7 +32097,7 @@
       </c>
       <c r="G616" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H616" t="inlineStr">
@@ -32157,7 +32157,7 @@
       </c>
       <c r="G617" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H617" t="inlineStr">
@@ -32209,7 +32209,7 @@
       </c>
       <c r="G618" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H618" t="inlineStr">
@@ -32261,7 +32261,7 @@
       </c>
       <c r="G619" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H619" t="inlineStr">
@@ -32485,7 +32485,7 @@
       </c>
       <c r="G623" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H623" t="inlineStr">
@@ -32644,7 +32644,7 @@
       </c>
       <c r="G626" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H626" t="inlineStr">
@@ -33102,7 +33102,7 @@
       </c>
       <c r="G635" t="inlineStr">
         <is>
-          <t>Lake Minara</t>
+          <t>Lago Minara</t>
         </is>
       </c>
       <c r="H635" t="inlineStr">
@@ -33154,7 +33154,7 @@
       </c>
       <c r="G636" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H636" t="inlineStr">
@@ -33361,7 +33361,7 @@
       </c>
       <c r="G640" t="inlineStr">
         <is>
-          <t>Lake Minara</t>
+          <t>Lago Minara</t>
         </is>
       </c>
       <c r="H640" t="inlineStr">
@@ -33513,7 +33513,7 @@
       </c>
       <c r="G643" t="inlineStr">
         <is>
-          <t>Lake Minara</t>
+          <t>Lago Minara</t>
         </is>
       </c>
       <c r="H643" t="inlineStr">
@@ -33674,7 +33674,7 @@
       </c>
       <c r="G646" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H646" t="inlineStr">
@@ -33888,7 +33888,7 @@
       </c>
       <c r="G650" t="inlineStr">
         <is>
-          <t>Lake Minara</t>
+          <t>Lago Minara</t>
         </is>
       </c>
       <c r="H650" t="inlineStr">
@@ -33995,7 +33995,7 @@
       </c>
       <c r="G652" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H652" t="inlineStr">
@@ -34097,7 +34097,7 @@
       </c>
       <c r="G654" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H654" t="inlineStr">
@@ -34149,7 +34149,7 @@
       </c>
       <c r="G655" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H655" t="inlineStr">
@@ -34313,7 +34313,7 @@
       </c>
       <c r="G658" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H658" t="inlineStr">
@@ -34612,7 +34612,7 @@
       </c>
       <c r="G664" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H664" t="inlineStr">
@@ -34936,7 +34936,7 @@
       </c>
       <c r="G670" t="inlineStr">
         <is>
-          <t>Lake Minara</t>
+          <t>Lago Minara</t>
         </is>
       </c>
       <c r="H670" t="inlineStr">
@@ -35040,7 +35040,7 @@
       </c>
       <c r="G672" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H672" t="inlineStr">
@@ -35194,7 +35194,7 @@
       </c>
       <c r="G675" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H675" t="inlineStr">
@@ -35249,7 +35249,7 @@
       </c>
       <c r="G676" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H676" t="inlineStr">
@@ -35457,7 +35457,7 @@
       </c>
       <c r="G680" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H680" t="inlineStr">
@@ -35604,7 +35604,7 @@
       </c>
       <c r="G683" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H683" t="inlineStr">
@@ -36017,7 +36017,7 @@
       </c>
       <c r="G691" t="inlineStr">
         <is>
-          <t>Lake Minara</t>
+          <t>Lago Minara</t>
         </is>
       </c>
       <c r="H691" t="inlineStr">
@@ -36132,7 +36132,7 @@
       </c>
       <c r="G693" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H693" t="inlineStr">
@@ -36294,7 +36294,7 @@
       </c>
       <c r="G696" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H696" t="inlineStr">
@@ -36404,7 +36404,7 @@
       </c>
       <c r="G698" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H698" t="inlineStr">
@@ -36613,7 +36613,7 @@
       </c>
       <c r="G702" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H702" t="inlineStr">
@@ -36720,7 +36720,7 @@
       </c>
       <c r="G704" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H704" t="inlineStr">
@@ -36932,7 +36932,7 @@
       </c>
       <c r="G708" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H708" t="inlineStr">
@@ -37081,7 +37081,7 @@
       </c>
       <c r="G711" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H711" t="inlineStr">
@@ -37304,7 +37304,7 @@
       </c>
       <c r="G716" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H716" t="inlineStr">
@@ -37399,7 +37399,7 @@
       </c>
       <c r="G718" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H718" t="inlineStr">
@@ -37496,7 +37496,7 @@
       </c>
       <c r="G720" t="inlineStr">
         <is>
-          <t>Lake Minara</t>
+          <t>Lago Minara</t>
         </is>
       </c>
       <c r="H720" t="inlineStr">
@@ -37533,7 +37533,7 @@
       </c>
       <c r="G721" t="inlineStr">
         <is>
-          <t>Lake Minara</t>
+          <t>Lago Minara</t>
         </is>
       </c>
       <c r="H721" t="inlineStr">
@@ -37845,7 +37845,7 @@
       </c>
       <c r="G727" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H727" t="inlineStr">
@@ -38216,7 +38216,7 @@
       </c>
       <c r="G734" t="inlineStr">
         <is>
-          <t>Lake Minara</t>
+          <t>Lago Minara</t>
         </is>
       </c>
       <c r="H734" t="inlineStr">
@@ -38462,7 +38462,7 @@
       </c>
       <c r="G739" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H739" t="inlineStr">
@@ -38671,7 +38671,7 @@
       </c>
       <c r="G743" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H743" t="inlineStr">
@@ -38768,7 +38768,7 @@
       </c>
       <c r="G745" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H745" t="inlineStr">
@@ -38815,7 +38815,7 @@
       </c>
       <c r="G746" t="inlineStr">
         <is>
-          <t>Lake Minara</t>
+          <t>Lago Minara</t>
         </is>
       </c>
       <c r="H746" t="inlineStr">
@@ -38852,7 +38852,7 @@
       </c>
       <c r="G747" t="inlineStr">
         <is>
-          <t>Lake Minara</t>
+          <t>Lago Minara</t>
         </is>
       </c>
       <c r="H747" t="inlineStr">
@@ -38998,7 +38998,7 @@
       </c>
       <c r="G750" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H750" t="inlineStr">
@@ -39038,7 +39038,7 @@
       </c>
       <c r="G751" t="inlineStr">
         <is>
-          <t>Lake Minara</t>
+          <t>Lago Minara</t>
         </is>
       </c>
       <c r="H751" t="inlineStr">
@@ -39289,7 +39289,7 @@
       </c>
       <c r="G756" t="inlineStr">
         <is>
-          <t>Lake Minara</t>
+          <t>Lago Minara</t>
         </is>
       </c>
       <c r="H756" t="inlineStr">
@@ -39329,7 +39329,7 @@
       </c>
       <c r="G757" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H757" t="inlineStr">
@@ -39540,7 +39540,7 @@
       </c>
       <c r="G761" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H761" t="inlineStr">
@@ -40441,7 +40441,7 @@
       </c>
       <c r="G778" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H778" t="inlineStr">
@@ -40496,7 +40496,7 @@
       </c>
       <c r="G779" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H779" t="inlineStr">
@@ -40546,7 +40546,7 @@
       </c>
       <c r="G780" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H780" t="inlineStr">
@@ -40745,7 +40745,7 @@
       </c>
       <c r="G784" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H784" t="inlineStr">
@@ -41115,7 +41115,7 @@
       </c>
       <c r="G791" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H791" t="inlineStr">
@@ -41581,7 +41581,7 @@
       </c>
       <c r="G800" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H800" t="inlineStr">
@@ -41788,7 +41788,7 @@
       </c>
       <c r="G804" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H804" t="inlineStr">
@@ -41835,7 +41835,7 @@
       </c>
       <c r="G805" t="inlineStr">
         <is>
-          <t>Lake Minara</t>
+          <t>Lago Minara</t>
         </is>
       </c>
       <c r="H805" t="inlineStr">
@@ -42192,7 +42192,7 @@
       </c>
       <c r="G812" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H812" t="inlineStr">
@@ -42247,7 +42247,7 @@
       </c>
       <c r="G813" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H813" t="inlineStr">
@@ -42341,7 +42341,7 @@
       </c>
       <c r="G815" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H815" t="inlineStr">
@@ -42620,7 +42620,7 @@
       </c>
       <c r="G820" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H820" t="inlineStr">
@@ -42784,7 +42784,7 @@
       </c>
       <c r="G823" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H823" t="inlineStr">
@@ -43105,7 +43105,7 @@
       </c>
       <c r="G829" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H829" t="inlineStr">
@@ -43160,7 +43160,7 @@
       </c>
       <c r="G830" t="inlineStr">
         <is>
-          <t>Lake Minara</t>
+          <t>Lago Minara</t>
         </is>
       </c>
       <c r="H830" t="inlineStr">
@@ -43456,7 +43456,7 @@
       </c>
       <c r="G836" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H836" t="inlineStr">
@@ -43665,7 +43665,7 @@
       </c>
       <c r="G840" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H840" t="inlineStr">
@@ -43942,7 +43942,7 @@
       </c>
       <c r="G845" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H845" t="inlineStr">
@@ -44287,7 +44287,7 @@
       </c>
       <c r="G852" t="inlineStr">
         <is>
-          <t>Lake Minara</t>
+          <t>Lago Minara</t>
         </is>
       </c>
       <c r="H852" t="inlineStr">
@@ -44332,7 +44332,7 @@
       </c>
       <c r="G853" t="inlineStr">
         <is>
-          <t>Lake Minara</t>
+          <t>Lago Minara</t>
         </is>
       </c>
       <c r="H853" t="inlineStr">
@@ -44389,7 +44389,7 @@
       </c>
       <c r="G854" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H854" t="inlineStr">
@@ -45066,7 +45066,7 @@
       </c>
       <c r="G867" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H867" t="inlineStr">
@@ -45126,7 +45126,7 @@
       </c>
       <c r="G868" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H868" t="inlineStr">
@@ -45397,7 +45397,7 @@
       </c>
       <c r="G873" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H873" t="inlineStr">
@@ -45509,7 +45509,7 @@
       </c>
       <c r="G875" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H875" t="inlineStr">
@@ -45660,7 +45660,7 @@
       </c>
       <c r="G878" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H878" t="inlineStr">
@@ -45982,7 +45982,7 @@
       </c>
       <c r="G884" t="inlineStr">
         <is>
-          <t>Lake Minara</t>
+          <t>Lago Minara</t>
         </is>
       </c>
       <c r="H884" t="inlineStr">
@@ -46194,7 +46194,7 @@
       </c>
       <c r="G888" t="inlineStr">
         <is>
-          <t>Lake Minara</t>
+          <t>Lago Minara</t>
         </is>
       </c>
       <c r="H888" t="inlineStr">
@@ -46447,7 +46447,7 @@
       </c>
       <c r="G893" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H893" t="inlineStr">
@@ -46695,7 +46695,7 @@
       </c>
       <c r="G898" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H898" t="inlineStr">
@@ -46740,7 +46740,7 @@
       </c>
       <c r="G899" t="inlineStr">
         <is>
-          <t>LAKE MINARA</t>
+          <t>LAGO MINARA</t>
         </is>
       </c>
       <c r="H899" t="inlineStr">
@@ -47100,7 +47100,7 @@
       </c>
       <c r="G906" t="inlineStr">
         <is>
-          <t>Lake Minara</t>
+          <t>Lago Minara</t>
         </is>
       </c>
       <c r="H906" t="inlineStr">

</xml_diff>